<commit_message>
Update prior meeting with CNA:     * RBS-TargetsAnalysis-CNA.xlsx: cheked for effect of changing Al entrance energy for the Sn exit energy, instead of the incident beam energy; calibration parameters change; look up new stopping power values; thicknesses slighly change; calibration parameters seem to better match the ones from SimNRA; only did it for the 3.2 MeV run, need to do it for the others; changed spreadsheet layout;
</commit_message>
<xml_diff>
--- a/Tuning.xlsx
+++ b/Tuning.xlsx
@@ -82,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -344,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -398,27 +398,99 @@
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -428,72 +500,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -506,27 +527,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -823,28 +827,30 @@
     <col min="16" max="16" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q1" s="74"/>
+    </row>
     <row r="2" spans="2:17" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="61" t="s">
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="58" t="s">
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="10" t="s">
@@ -859,19 +865,19 @@
       <c r="F3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="11"/>
@@ -884,18 +890,18 @@
       <c r="O3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
     </row>
     <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="61" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="51"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="27" t="s">
         <v>15</v>
       </c>
@@ -905,28 +911,28 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="67">
+      <c r="C5" s="62"/>
+      <c r="D5" s="53">
         <v>275000</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="36">
         <v>0.127</v>
       </c>
       <c r="F5" s="22">
         <v>2170000</v>
       </c>
-      <c r="G5" s="66">
-        <f>F5/F6</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="68">
+      <c r="G5" s="59">
+        <f>D5/D6</f>
+        <v>4.6063651591289778</v>
+      </c>
+      <c r="H5" s="54">
         <v>4190</v>
       </c>
       <c r="I5" s="29">
@@ -935,45 +941,48 @@
       <c r="J5" s="29">
         <v>2240000</v>
       </c>
-      <c r="K5" s="30">
-        <f>J5/J6</f>
-        <v>1.1727748691099475</v>
+      <c r="K5" s="60">
+        <f>H5/H6</f>
+        <v>9.4796380090497738</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="12">
         <f>F5/J5</f>
         <v>0.96875</v>
       </c>
-      <c r="N5" s="69">
+      <c r="N5" s="55">
         <f>D5/H5</f>
         <v>65.632458233890219</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="49">
         <f>E5/I5</f>
         <v>67.914438502673804</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="58">
         <f>N5-O5</f>
         <v>-2.2819802687835846</v>
       </c>
-      <c r="Q5" s="49"/>
+      <c r="Q5" s="73">
+        <f>I5/I6</f>
+        <v>8.0603448275862064</v>
+      </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="67">
+      <c r="C6" s="62"/>
+      <c r="D6" s="53">
         <v>59700</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="36">
         <v>2.75E-2</v>
       </c>
       <c r="F6" s="22">
         <v>2170000</v>
       </c>
-      <c r="G6" s="66"/>
-      <c r="H6" s="68">
+      <c r="G6" s="59"/>
+      <c r="H6" s="54">
         <v>442</v>
       </c>
       <c r="I6" s="29">
@@ -982,83 +991,83 @@
       <c r="J6" s="29">
         <v>1910000</v>
       </c>
-      <c r="K6" s="30"/>
+      <c r="K6" s="60"/>
       <c r="L6" s="6"/>
       <c r="M6" s="12">
         <f>F6/J6</f>
         <v>1.1361256544502618</v>
       </c>
-      <c r="N6" s="69">
+      <c r="N6" s="55">
         <f>D6/H6</f>
         <v>135.06787330316743</v>
       </c>
-      <c r="O6" s="53">
+      <c r="O6" s="49">
         <f>E6/I6</f>
         <v>118.53448275862068</v>
       </c>
-      <c r="P6" s="72">
+      <c r="P6" s="58">
         <f>N6-O6</f>
         <v>16.533390544546748</v>
       </c>
-      <c r="Q6" s="49"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="15"/>
-      <c r="C7" s="39"/>
+      <c r="C7" s="63"/>
       <c r="D7" s="23"/>
       <c r="E7" s="26"/>
       <c r="F7" s="24"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="61" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="21"/>
-      <c r="E8" s="40"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="67">
+      <c r="C9" s="62"/>
+      <c r="D9" s="53">
         <v>1250000</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="36">
         <v>0.1268</v>
       </c>
       <c r="F9" s="22">
         <v>9850000</v>
       </c>
-      <c r="G9" s="66">
-        <f>F9/F10</f>
-        <v>0.98598598598598597</v>
-      </c>
-      <c r="H9" s="68">
+      <c r="G9" s="59">
+        <f>D9/D10</f>
+        <v>4.562043795620438</v>
+      </c>
+      <c r="H9" s="54">
         <v>16800</v>
       </c>
       <c r="I9" s="29">
@@ -1067,45 +1076,48 @@
       <c r="J9" s="29">
         <v>8970000</v>
       </c>
-      <c r="K9" s="30">
-        <f>J9/J10</f>
-        <v>1.0515826494724503</v>
+      <c r="K9" s="60">
+        <f>H9/H10</f>
+        <v>8.527918781725889</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="12">
         <f>F9/J9</f>
         <v>1.0981047937569677</v>
       </c>
-      <c r="N9" s="69">
+      <c r="N9" s="55">
         <f>D9/H9</f>
         <v>74.404761904761898</v>
       </c>
-      <c r="O9" s="53">
+      <c r="O9" s="49">
         <f>E9/I9</f>
         <v>67.807486631016047</v>
       </c>
-      <c r="P9" s="72">
+      <c r="P9" s="58">
         <f>N9-O9</f>
         <v>6.5972752737458507</v>
       </c>
-      <c r="Q9" s="49"/>
+      <c r="Q9" s="73">
+        <f>I9/I10</f>
+        <v>8.0952380952380949</v>
+      </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="67">
+      <c r="C10" s="62"/>
+      <c r="D10" s="53">
         <v>274000</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="36">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="F10" s="22">
         <v>9990000</v>
       </c>
-      <c r="G10" s="66"/>
-      <c r="H10" s="68">
+      <c r="G10" s="59"/>
+      <c r="H10" s="54">
         <v>1970</v>
       </c>
       <c r="I10" s="29">
@@ -1114,83 +1126,83 @@
       <c r="J10" s="29">
         <v>8530000</v>
       </c>
-      <c r="K10" s="30"/>
+      <c r="K10" s="60"/>
       <c r="L10" s="6"/>
       <c r="M10" s="12">
         <f>F10/J10</f>
         <v>1.1711606096131302</v>
       </c>
-      <c r="N10" s="69">
+      <c r="N10" s="55">
         <f>D10/H10</f>
         <v>139.08629441624365</v>
       </c>
-      <c r="O10" s="53">
+      <c r="O10" s="49">
         <f>E10/I10</f>
         <v>118.61471861471861</v>
       </c>
-      <c r="P10" s="72">
+      <c r="P10" s="58">
         <f>N10-O10</f>
         <v>20.471575801525034</v>
       </c>
-      <c r="Q10" s="49"/>
+      <c r="Q10" s="45"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="7"/>
-      <c r="C11" s="39"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="21"/>
-      <c r="E11" s="40"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="61" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="51"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="33"/>
+      <c r="K12" s="32"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="67">
+      <c r="C13" s="62"/>
+      <c r="D13" s="53">
         <v>2790000</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="36">
         <v>0.12670000000000001</v>
       </c>
       <c r="F13" s="22">
         <v>22000000</v>
       </c>
-      <c r="G13" s="66">
-        <f>F13/F14</f>
-        <v>0.9821428571428571</v>
-      </c>
-      <c r="H13" s="68">
+      <c r="G13" s="59">
+        <f>D13/D14</f>
+        <v>4.5365853658536581</v>
+      </c>
+      <c r="H13" s="54">
         <v>41600</v>
       </c>
       <c r="I13" s="29">
@@ -1199,45 +1211,48 @@
       <c r="J13" s="29">
         <v>22200000</v>
       </c>
-      <c r="K13" s="30">
-        <f>J13/J14</f>
-        <v>0.99551569506726456</v>
+      <c r="K13" s="60">
+        <f>H13/H14</f>
+        <v>7.9846449136276387</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="12">
         <f>F13/J13</f>
         <v>0.99099099099099097</v>
       </c>
-      <c r="N13" s="69">
+      <c r="N13" s="55">
         <f>D13/H13</f>
         <v>67.067307692307693</v>
       </c>
-      <c r="O13" s="53">
+      <c r="O13" s="49">
         <f>E13/I13</f>
         <v>67.393617021276597</v>
       </c>
-      <c r="P13" s="72">
+      <c r="P13" s="58">
         <f>N13-O13</f>
         <v>-0.32630932896890386</v>
       </c>
-      <c r="Q13" s="49"/>
+      <c r="Q13" s="73">
+        <f>I13/I14</f>
+        <v>8.0686695278969953</v>
+      </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="67">
+      <c r="C14" s="62"/>
+      <c r="D14" s="53">
         <v>615000</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="36">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="F14" s="22">
         <v>22400000</v>
       </c>
-      <c r="G14" s="66"/>
-      <c r="H14" s="68">
+      <c r="G14" s="59"/>
+      <c r="H14" s="54">
         <v>5210</v>
       </c>
       <c r="I14" s="29">
@@ -1246,83 +1261,83 @@
       <c r="J14" s="29">
         <v>22300000</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="60"/>
       <c r="L14" s="6"/>
       <c r="M14" s="12">
         <f>F14/J14</f>
         <v>1.0044843049327354</v>
       </c>
-      <c r="N14" s="69">
+      <c r="N14" s="55">
         <f>D14/H14</f>
         <v>118.04222648752399</v>
       </c>
-      <c r="O14" s="53">
+      <c r="O14" s="49">
         <f>E14/I14</f>
         <v>117.59656652360515</v>
       </c>
-      <c r="P14" s="72">
+      <c r="P14" s="58">
         <f>N14-O14</f>
         <v>0.44565996391884255</v>
       </c>
-      <c r="Q14" s="49"/>
+      <c r="Q14" s="45"/>
     </row>
     <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="5"/>
-      <c r="C15" s="39"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="23"/>
       <c r="E15" s="26"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="53"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="61" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="21"/>
-      <c r="E16" s="40"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="22"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="49"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="67">
+      <c r="C17" s="62"/>
+      <c r="D17" s="53">
         <v>5240000</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="36">
         <v>0.1268</v>
       </c>
       <c r="F17" s="22">
         <v>41300000</v>
       </c>
-      <c r="G17" s="66">
-        <f>F17/F18</f>
-        <v>0.98333333333333328</v>
-      </c>
-      <c r="H17" s="68">
+      <c r="G17" s="59">
+        <f>D17/D18</f>
+        <v>4.5565217391304351</v>
+      </c>
+      <c r="H17" s="54">
         <v>81800</v>
       </c>
       <c r="I17" s="29">
@@ -1331,45 +1346,48 @@
       <c r="J17" s="29">
         <v>43600000</v>
       </c>
-      <c r="K17" s="30">
-        <f>J17/J18</f>
-        <v>0.94577006507592187</v>
+      <c r="K17" s="60">
+        <f>H17/H18</f>
+        <v>7.6448598130841123</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="12">
         <f>F17/J17</f>
         <v>0.94724770642201839</v>
       </c>
-      <c r="N17" s="69">
+      <c r="N17" s="55">
         <f>D17/H17</f>
         <v>64.058679706601467</v>
       </c>
-      <c r="O17" s="53">
+      <c r="O17" s="49">
         <f>E17/I17</f>
         <v>67.446808510638292</v>
       </c>
-      <c r="P17" s="72">
+      <c r="P17" s="58">
         <f>N17-O17</f>
         <v>-3.3881288040368247</v>
       </c>
-      <c r="Q17" s="49"/>
+      <c r="Q17" s="73">
+        <f>I17/I18</f>
+        <v>8.1034482758620694</v>
+      </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="67">
+      <c r="C18" s="62"/>
+      <c r="D18" s="53">
         <v>1150000</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="36">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="F18" s="22">
         <v>42000000</v>
       </c>
-      <c r="G18" s="66"/>
-      <c r="H18" s="68">
+      <c r="G18" s="59"/>
+      <c r="H18" s="54">
         <v>10700</v>
       </c>
       <c r="I18" s="29">
@@ -1378,83 +1396,83 @@
       <c r="J18" s="29">
         <v>46100000</v>
       </c>
-      <c r="K18" s="30"/>
+      <c r="K18" s="60"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12">
         <f>F18/J18</f>
         <v>0.91106290672451196</v>
       </c>
-      <c r="N18" s="69">
+      <c r="N18" s="55">
         <f>D18/H18</f>
         <v>107.4766355140187</v>
       </c>
-      <c r="O18" s="53">
+      <c r="O18" s="49">
         <f>E18/I18</f>
         <v>118.10344827586208</v>
       </c>
-      <c r="P18" s="72">
+      <c r="P18" s="58">
         <f>N18-O18</f>
         <v>-10.626812761843382</v>
       </c>
-      <c r="Q18" s="49"/>
+      <c r="Q18" s="45"/>
     </row>
     <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="7"/>
-      <c r="C19" s="39"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="40"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="35"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="61" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="20"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="51"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
-      <c r="K20" s="33"/>
+      <c r="K20" s="32"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="67">
+      <c r="C21" s="62"/>
+      <c r="D21" s="53">
         <v>10200000</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="36">
         <v>0.12690000000000001</v>
       </c>
       <c r="F21" s="22">
         <v>80800000</v>
       </c>
-      <c r="G21" s="66">
-        <f>F21/F22</f>
-        <v>0.98058252427184467</v>
-      </c>
-      <c r="H21" s="68">
+      <c r="G21" s="59">
+        <f>D21/D22</f>
+        <v>4.5132743362831862</v>
+      </c>
+      <c r="H21" s="54">
         <v>170000</v>
       </c>
       <c r="I21" s="29">
@@ -1463,45 +1481,48 @@
       <c r="J21" s="29">
         <v>90600000</v>
       </c>
-      <c r="K21" s="30">
-        <f>J21/J22</f>
-        <v>0.95670538542766637</v>
+      <c r="K21" s="60">
+        <f>H21/H22</f>
+        <v>7.6923076923076925</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="12">
         <f>F21/J21</f>
         <v>0.89183222958057395</v>
       </c>
-      <c r="N21" s="69">
+      <c r="N21" s="55">
         <f>D21/H21</f>
         <v>60</v>
       </c>
-      <c r="O21" s="53">
+      <c r="O21" s="49">
         <f>E21/I21</f>
         <v>67.860962566844933</v>
       </c>
-      <c r="P21" s="72">
+      <c r="P21" s="58">
         <f>N21-O21</f>
         <v>-7.8609625668449326</v>
       </c>
-      <c r="Q21" s="49"/>
+      <c r="Q21" s="73">
+        <f>I21/I22</f>
+        <v>8.0257510729613735</v>
+      </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="67">
+      <c r="C22" s="62"/>
+      <c r="D22" s="53">
         <v>2260000</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="36">
         <v>2.75E-2</v>
       </c>
       <c r="F22" s="22">
         <v>82400000</v>
       </c>
-      <c r="G22" s="66"/>
-      <c r="H22" s="68">
+      <c r="G22" s="59"/>
+      <c r="H22" s="54">
         <v>22100</v>
       </c>
       <c r="I22" s="29">
@@ -1510,83 +1531,83 @@
       <c r="J22" s="29">
         <v>94700000</v>
       </c>
-      <c r="K22" s="30"/>
+      <c r="K22" s="60"/>
       <c r="L22" s="6"/>
       <c r="M22" s="12">
         <f>F22/J22</f>
         <v>0.87011615628299899</v>
       </c>
-      <c r="N22" s="69">
+      <c r="N22" s="55">
         <f>D22/H22</f>
         <v>102.26244343891403</v>
       </c>
-      <c r="O22" s="53">
+      <c r="O22" s="49">
         <f>E22/I22</f>
         <v>118.02575107296137</v>
       </c>
-      <c r="P22" s="72">
+      <c r="P22" s="58">
         <f>N22-O22</f>
         <v>-15.763307634047337</v>
       </c>
-      <c r="Q22" s="49"/>
+      <c r="Q22" s="45"/>
     </row>
     <row r="23" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="5"/>
-      <c r="C23" s="39"/>
+      <c r="C23" s="63"/>
       <c r="D23" s="23"/>
       <c r="E23" s="26"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="71"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="49"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B24" s="13"/>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="61" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="22"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="35"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="34"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B25" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="67">
+      <c r="C25" s="62"/>
+      <c r="D25" s="53">
         <v>19900000</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="36">
         <v>0.1268</v>
       </c>
       <c r="F25" s="22">
         <v>157000000</v>
       </c>
-      <c r="G25" s="66">
-        <f>F25/F26</f>
-        <v>0.96319018404907975</v>
-      </c>
-      <c r="H25" s="68">
+      <c r="G25" s="59">
+        <f>D25/D26</f>
+        <v>4.4519015659955254</v>
+      </c>
+      <c r="H25" s="54">
         <v>358000</v>
       </c>
       <c r="I25" s="29">
@@ -1595,45 +1616,48 @@
       <c r="J25" s="29">
         <v>191000000</v>
       </c>
-      <c r="K25" s="30">
-        <f>J25/J26</f>
-        <v>0.95499999999999996</v>
+      <c r="K25" s="60">
+        <f>H25/H26</f>
+        <v>7.698924731182796</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="12">
         <f>F25/J25</f>
         <v>0.82198952879581155</v>
       </c>
-      <c r="N25" s="69">
+      <c r="N25" s="55">
         <f>D25/H25</f>
         <v>55.58659217877095</v>
       </c>
-      <c r="O25" s="53">
+      <c r="O25" s="49">
         <f>E25/I25</f>
         <v>67.807486631016047</v>
       </c>
-      <c r="P25" s="72">
+      <c r="P25" s="58">
         <f>N25-O25</f>
         <v>-12.220894452245098</v>
       </c>
-      <c r="Q25" s="49"/>
+      <c r="Q25" s="73">
+        <f>I25/I26</f>
+        <v>8.0257510729613735</v>
+      </c>
     </row>
     <row r="26" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="67">
+      <c r="C26" s="62"/>
+      <c r="D26" s="53">
         <v>4470000</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="36">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="F26" s="22">
         <v>163000000</v>
       </c>
-      <c r="G26" s="66"/>
-      <c r="H26" s="68">
+      <c r="G26" s="59"/>
+      <c r="H26" s="54">
         <v>46500</v>
       </c>
       <c r="I26" s="29">
@@ -1642,42 +1666,42 @@
       <c r="J26" s="29">
         <v>200000000</v>
       </c>
-      <c r="K26" s="30"/>
+      <c r="K26" s="60"/>
       <c r="L26" s="6"/>
       <c r="M26" s="12">
         <f>F26/J26</f>
         <v>0.81499999999999995</v>
       </c>
-      <c r="N26" s="69">
+      <c r="N26" s="55">
         <f>D26/H26</f>
         <v>96.129032258064512</v>
       </c>
-      <c r="O26" s="53">
+      <c r="O26" s="49">
         <f>E26/I26</f>
         <v>117.59656652360515</v>
       </c>
-      <c r="P26" s="72">
+      <c r="P26" s="58">
         <f>N26-O26</f>
         <v>-21.467534265540635</v>
       </c>
-      <c r="Q26" s="49"/>
+      <c r="Q26" s="45"/>
     </row>
     <row r="27" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="39"/>
+      <c r="C27" s="63"/>
       <c r="D27" s="23"/>
       <c r="E27" s="26"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="36"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="35"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.35">
       <c r="D30" s="1"/>
@@ -1687,14 +1711,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K25:K26"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="L2:O2"/>
@@ -1708,6 +1724,14 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C16:C19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K25:K26"/>
   </mergeCells>
   <conditionalFormatting sqref="M4:M27">
     <cfRule type="colorScale" priority="1">

</xml_diff>